<commit_message>
städat kod och fixat praat values för emotions
</commit_message>
<xml_diff>
--- a/exports/segment_level_id_0043_neg_anger_analysis.xlsx
+++ b/exports/segment_level_id_0043_neg_anger_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Segment Mid Time (s)</t>
+          <t>time</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -452,6 +452,11 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Hume anger Score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Praat Label</t>
         </is>
       </c>
     </row>
@@ -460,13 +465,18 @@
         <v>1.707877978</v>
       </c>
       <c r="B2" t="n">
-        <v>218.2922666866691</v>
+        <v>191.6896484019795</v>
       </c>
       <c r="C2" t="n">
-        <v>59.13108270560521</v>
+        <v>61.18225459059844</v>
       </c>
       <c r="D2" t="n">
         <v>0.716</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -474,13 +484,18 @@
         <v>4.1643026</v>
       </c>
       <c r="B3" t="n">
-        <v>207.0144162486189</v>
+        <v>231.8624386244848</v>
       </c>
       <c r="C3" t="n">
-        <v>58.73199163770558</v>
+        <v>52.53484972441996</v>
       </c>
       <c r="D3" t="n">
         <v>0.38</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -488,13 +503,18 @@
         <v>5.26270365</v>
       </c>
       <c r="B4" t="n">
-        <v>209.5964867250489</v>
+        <v>233.5510455051854</v>
       </c>
       <c r="C4" t="n">
-        <v>59.19221801610243</v>
+        <v>65.27336074361563</v>
       </c>
       <c r="D4" t="n">
         <v>0.731</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -502,13 +522,18 @@
         <v>7.43953525</v>
       </c>
       <c r="B5" t="n">
-        <v>209.5815958061352</v>
+        <v>177.2476450762052</v>
       </c>
       <c r="C5" t="n">
-        <v>59.59399880644404</v>
+        <v>65.77709160669976</v>
       </c>
       <c r="D5" t="n">
         <v>0.225</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -516,13 +541,18 @@
         <v>11.2939245</v>
       </c>
       <c r="B6" t="n">
-        <v>202.9448327587775</v>
+        <v>185.882137541738</v>
       </c>
       <c r="C6" t="n">
-        <v>59.08403466251082</v>
+        <v>57.21560925996133</v>
       </c>
       <c r="D6" t="n">
         <v>0.151</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -530,13 +560,18 @@
         <v>15.325</v>
       </c>
       <c r="B7" t="n">
-        <v>207.130590045841</v>
+        <v>216.4374150207751</v>
       </c>
       <c r="C7" t="n">
-        <v>56.91221092519223</v>
+        <v>61.3490178925293</v>
       </c>
       <c r="D7" t="n">
         <v>0.289</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -544,13 +579,18 @@
         <v>17.925</v>
       </c>
       <c r="B8" t="n">
-        <v>214.5811728839418</v>
+        <v>167.4480746313774</v>
       </c>
       <c r="C8" t="n">
-        <v>57.22591729894543</v>
+        <v>54.70533428075144</v>
       </c>
       <c r="D8" t="n">
         <v>0.659</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -558,13 +598,18 @@
         <v>21.525</v>
       </c>
       <c r="B9" t="n">
-        <v>224.4256315104169</v>
+        <v>201.8726402485668</v>
       </c>
       <c r="C9" t="n">
-        <v>55.30538863868622</v>
+        <v>66.29160810830206</v>
       </c>
       <c r="D9" t="n">
         <v>0.504</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -572,13 +617,18 @@
         <v>23.305</v>
       </c>
       <c r="B10" t="n">
-        <v>230.9866963372931</v>
+        <v>245.6079890769943</v>
       </c>
       <c r="C10" t="n">
-        <v>55.44752475267376</v>
+        <v>53.22962207934772</v>
       </c>
       <c r="D10" t="n">
         <v>0.315</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -586,13 +636,18 @@
         <v>25.025</v>
       </c>
       <c r="B11" t="n">
-        <v>239.337930763798</v>
+        <v>233.823800445258</v>
       </c>
       <c r="C11" t="n">
-        <v>58.83195199142133</v>
+        <v>53.27962219302967</v>
       </c>
       <c r="D11" t="n">
         <v>0.242</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -600,13 +655,18 @@
         <v>29.9567595</v>
       </c>
       <c r="B12" t="n">
-        <v>240.5446192664371</v>
+        <v>247.3240934338943</v>
       </c>
       <c r="C12" t="n">
-        <v>58.37312883227449</v>
+        <v>65.58672811893763</v>
       </c>
       <c r="D12" t="n">
         <v>0.371</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -614,13 +674,18 @@
         <v>33.4339</v>
       </c>
       <c r="B13" t="n">
-        <v>226.9353448142706</v>
+        <v>208.1576955976502</v>
       </c>
       <c r="C13" t="n">
-        <v>61.85902297765219</v>
+        <v>58.33563423240206</v>
       </c>
       <c r="D13" t="n">
         <v>0.591</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -628,13 +693,18 @@
         <v>36.21161</v>
       </c>
       <c r="B14" t="n">
-        <v>219.9255613728877</v>
+        <v>201.3080359845419</v>
       </c>
       <c r="C14" t="n">
-        <v>59.77960057580674</v>
+        <v>68.31256952537977</v>
       </c>
       <c r="D14" t="n">
         <v>0.473</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -642,13 +712,18 @@
         <v>39.825003</v>
       </c>
       <c r="B15" t="n">
-        <v>223.3846323772712</v>
+        <v>248.6866536445313</v>
       </c>
       <c r="C15" t="n">
-        <v>64.67748494785431</v>
+        <v>65.39013064218855</v>
       </c>
       <c r="D15" t="n">
         <v>0.169</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -656,13 +731,18 @@
         <v>41.6850015</v>
       </c>
       <c r="B16" t="n">
-        <v>221.3345993544895</v>
+        <v>246.8835872138402</v>
       </c>
       <c r="C16" t="n">
-        <v>62.20951117769229</v>
+        <v>67.6579554849902</v>
       </c>
       <c r="D16" t="n">
         <v>0.514</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -670,13 +750,18 @@
         <v>43.965002</v>
       </c>
       <c r="B17" t="n">
-        <v>229.0883438395299</v>
+        <v>204.4413285475489</v>
       </c>
       <c r="C17" t="n">
-        <v>61.36481370153665</v>
+        <v>63.95552118291549</v>
       </c>
       <c r="D17" t="n">
         <v>0.136</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -684,13 +769,18 @@
         <v>47.045</v>
       </c>
       <c r="B18" t="n">
-        <v>238.3005697504232</v>
+        <v>236.9850972149102</v>
       </c>
       <c r="C18" t="n">
-        <v>61.37219879240529</v>
+        <v>66.84129124089847</v>
       </c>
       <c r="D18" t="n">
         <v>0.425</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -698,13 +788,18 @@
         <v>51.3450015</v>
       </c>
       <c r="B19" t="n">
-        <v>254.9613805795802</v>
+        <v>252.4475508835506</v>
       </c>
       <c r="C19" t="n">
-        <v>61.00511280035678</v>
+        <v>60.94675076648562</v>
       </c>
       <c r="D19" t="n">
         <v>0.477</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -712,13 +807,18 @@
         <v>56.6182965</v>
       </c>
       <c r="B20" t="n">
-        <v>239.1081140340122</v>
+        <v>227.1528452591361</v>
       </c>
       <c r="C20" t="n">
-        <v>60.56427338995028</v>
+        <v>70.48025136775708</v>
       </c>
       <c r="D20" t="n">
         <v>0.739</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -726,13 +826,18 @@
         <v>61.5748615</v>
       </c>
       <c r="B21" t="n">
-        <v>232.0751328565637</v>
+        <v>180.1942825438341</v>
       </c>
       <c r="C21" t="n">
-        <v>63.75978506778567</v>
+        <v>63.82513395829859</v>
       </c>
       <c r="D21" t="n">
         <v>0.219</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -740,13 +845,18 @@
         <v>64.52264750000001</v>
       </c>
       <c r="B22" t="n">
-        <v>235.9052587678797</v>
+        <v>227.5726412942738</v>
       </c>
       <c r="C22" t="n">
-        <v>66.70950316477902</v>
+        <v>70.85039711827095</v>
       </c>
       <c r="D22" t="n">
         <v>0.277</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -754,13 +864,18 @@
         <v>67.587705</v>
       </c>
       <c r="B23" t="n">
-        <v>242.1415267483479</v>
+        <v>239.7605994135779</v>
       </c>
       <c r="C23" t="n">
-        <v>69.6019068419302</v>
+        <v>68.40482233510463</v>
       </c>
       <c r="D23" t="n">
         <v>0.036</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -768,13 +883,18 @@
         <v>71.351145</v>
       </c>
       <c r="B24" t="n">
-        <v>233.7109281744931</v>
+        <v>255.4938470504626</v>
       </c>
       <c r="C24" t="n">
-        <v>70.29689586186765</v>
+        <v>69.31847242164309</v>
       </c>
       <c r="D24" t="n">
         <v>0.128</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -782,13 +902,18 @@
         <v>75.346003</v>
       </c>
       <c r="B25" t="n">
-        <v>221.5046608268993</v>
+        <v>220.8254725672719</v>
       </c>
       <c r="C25" t="n">
-        <v>67.95396708634009</v>
+        <v>70.437806301094</v>
       </c>
       <c r="D25" t="n">
         <v>0.593</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -796,13 +921,18 @@
         <v>79.56058300000001</v>
       </c>
       <c r="B26" t="n">
-        <v>221.021268344295</v>
+        <v>202.5392092414347</v>
       </c>
       <c r="C26" t="n">
-        <v>65.33363787139639</v>
+        <v>70.90531984436423</v>
       </c>
       <c r="D26" t="n">
         <v>0.08799999999999999</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -810,13 +940,18 @@
         <v>83.523157</v>
       </c>
       <c r="B27" t="n">
-        <v>234.4873763496899</v>
+        <v>231.7528436958735</v>
       </c>
       <c r="C27" t="n">
-        <v>64.45372049814277</v>
+        <v>64.27213797476745</v>
       </c>
       <c r="D27" t="n">
         <v>0.368</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -824,27 +959,35 @@
         <v>87.066642</v>
       </c>
       <c r="B28" t="n">
-        <v>234.1642973492984</v>
+        <v>248.5583206852246</v>
       </c>
       <c r="C28" t="n">
-        <v>60.54356259755998</v>
+        <v>65.56225596180012</v>
       </c>
       <c r="D28" t="n">
         <v>0.336</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>89.54400000000001</v>
       </c>
-      <c r="B29" t="n">
-        <v>234.6401290052869</v>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="n">
-        <v>58.77320371749381</v>
+        <v>48.72176356844336</v>
       </c>
       <c r="D29" t="n">
         <v>0.238</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -852,13 +995,18 @@
         <v>91.362065</v>
       </c>
       <c r="B30" t="n">
-        <v>233.0046748292549</v>
+        <v>155.3043119940262</v>
       </c>
       <c r="C30" t="n">
-        <v>57.04016297635336</v>
+        <v>53.09575079729106</v>
       </c>
       <c r="D30" t="n">
         <v>0.398</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -866,13 +1014,18 @@
         <v>92.77082999999999</v>
       </c>
       <c r="B31" t="n">
-        <v>221.1080662279303</v>
+        <v>225.1850319179004</v>
       </c>
       <c r="C31" t="n">
-        <v>54.83741784137622</v>
+        <v>57.61391680600597</v>
       </c>
       <c r="D31" t="n">
         <v>0.277</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>